<commit_message>
Updating external repo to match gatech repo.
</commit_message>
<xml_diff>
--- a/capstoneProj/PracticumProjectChecklist.xlsx
+++ b/capstoneProj/PracticumProjectChecklist.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="79">
   <si>
     <t>Pass</t>
   </si>
@@ -31,7 +31,7 @@
     <t>Testing Date</t>
   </si>
   <si>
-    <t>Looking for feedback on this format</t>
+    <t>We encourage app teams to update the checklist and Payload lists with language specific links and company policies to ensure future developers follow the companies requirements.</t>
   </si>
   <si>
     <t>Test app</t>
@@ -49,7 +49,7 @@
     <t>https://cheatsheetseries.owasp.org/cheatsheets/Error_Handling_Cheat_Sheet.html</t>
   </si>
   <si>
-    <t>Autocomplete disabled on sensitive input fields</t>
+    <t>Autocomplete Disabled on Sensitive Input Fields</t>
   </si>
   <si>
     <t>Emails, password, challenge questions, and other sensitive information should have autocomplete=off.</t>
@@ -58,7 +58,7 @@
     <t>https://www.w3schools.com/howto/howto_html_autocomplete_off.asp</t>
   </si>
   <si>
-    <t>Sensitive Information masked</t>
+    <t>Sensitive Information is Masked</t>
   </si>
   <si>
     <t>NPI should be masked to reduce shoulder surfing attacks.</t>
@@ -76,7 +76,7 @@
     <t>https://cwe.mitre.org/data/definitions/598.html</t>
   </si>
   <si>
-    <t>Unneccessary Methods Disabled</t>
+    <t>Unneccessary Methods are Disabled</t>
   </si>
   <si>
     <t>Do not allow unsafe methods such as Trace or Connect on any endpoint. Disable delete, post, etc if not needed on the endpoint.</t>
@@ -94,31 +94,190 @@
     <t>https://blog.matrixpost.net/redirect-from-http-to-https-using-the-iis-url-rewrite-module/</t>
   </si>
   <si>
-    <t>Response Headers</t>
-  </si>
-  <si>
-    <t>Caching</t>
-  </si>
-  <si>
-    <t>CSP</t>
-  </si>
-  <si>
-    <t>Cookie Attributes</t>
+    <t>Response Headers:</t>
+  </si>
+  <si>
+    <t>Content-Security-Policy</t>
+  </si>
+  <si>
+    <t>Does not include unsafe directives, wildcarded directives, or wildcards in subdomains.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>https://developer.mozilla.org/en-US/docs/Web/HTTP/Reference/Headers/Content-Security-Policy</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>https://csp-evaluator.withgoogle.com/</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>HSTS Response Header</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strict-Transport-Security: max-age=63072000; includeSubDomains; preload   Only use preload if external app. </t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/en-US/docs/Web/HTTP/Reference/Headers/Strict-Transport-Security</t>
+  </si>
+  <si>
+    <t>Caching Headers</t>
+  </si>
+  <si>
+    <t>Cache-Control: no-store. More lax: Expires: 0, Cache-Control: no-cache</t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/en-US/docs/Web/HTTP/Reference/Headers/Cache-Control
+https://www.rfc-editor.org/rfc/rfc9111.html</t>
+  </si>
+  <si>
+    <t>Information Leak Headers</t>
+  </si>
+  <si>
+    <t>Remove unneccessary headers, such as: Server, X-Powered-By,X-AspNet-Version.</t>
+  </si>
+  <si>
+    <t>https://support.waters.com/KB_Inf/Other/WKB202501_How_to_disable_the_Server_HTTP_header_in_Microsoft_IIS</t>
+  </si>
+  <si>
+    <t>CORS Headers</t>
+  </si>
+  <si>
+    <t>Do not set Access-Control-Allow-Origin to wildcard or reflect arbitrary origins/subdomains.</t>
+  </si>
+  <si>
+    <t>https://www.freecodecamp.org/news/exploiting-cors-guide-to-pentesting/#heading-exploitable-cors-cases</t>
+  </si>
+  <si>
+    <t>Cookies:</t>
   </si>
   <si>
     <t>HttpOnly</t>
   </si>
   <si>
-    <t>SameSite</t>
-  </si>
-  <si>
-    <t>Injections/Payloads Required</t>
-  </si>
-  <si>
-    <t>Login Page</t>
-  </si>
-  <si>
-    <t>Session Management</t>
+    <t>Prevents JavaScript from accessing the cookies(an easy target for XSS attacks)</t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/en-US/docs/Web/HTTP/Reference/Headers/Set-Cookie</t>
+  </si>
+  <si>
+    <t>Secure Flag</t>
+  </si>
+  <si>
+    <t>Prevents cookies from sending over HTTP.</t>
+  </si>
+  <si>
+    <t>SameSite Lax or Strict</t>
+  </si>
+  <si>
+    <t>SameSite cookies prevent cross-site attacks like CSRF. Lax: Cross-site requests will only send cookies in GET requests. Strict: Cookies will not send in any cross-site requests.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t xml:space="preserve">https://developer.mozilla.org/en-US/docs/Web/HTTP/Reference/Headers/Set-Cookie
+</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>https://portswigger.net/web-security/csrf/bypassing-samesite-restrictions</t>
+    </r>
+  </si>
+  <si>
+    <t>Narrow Path</t>
+  </si>
+  <si>
+    <t>Sensitive/session cookies must have a restrictive path set to prevent other applications on the same server from using this cookie.</t>
+  </si>
+  <si>
+    <t>https://owasp.org/www-project-web-security-testing-guide/latest/4-Web_Application_Security_Testing/06-Session_Management_Testing/02-Testing_for_Cookies_Attributes</t>
+  </si>
+  <si>
+    <t>Narrow Domain</t>
+  </si>
+  <si>
+    <t>Sensitive/session cookies must have the domain set to the subdomain when applicable.</t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/en-US/docs/Web/Security/Practical_implementation_guides/Cookies</t>
+  </si>
+  <si>
+    <t>Injections/Payloads Required:</t>
+  </si>
+  <si>
+    <t>Cross-Site Scripting(XSS)</t>
+  </si>
+  <si>
+    <t>SQL Injection</t>
+  </si>
+  <si>
+    <t>Directory Traversal</t>
+  </si>
+  <si>
+    <t>OS Command Injection</t>
+  </si>
+  <si>
+    <t>SQL Injection on Login Page</t>
+  </si>
+  <si>
+    <t>Login Page:</t>
+  </si>
+  <si>
+    <t>Weak Passwords Not Allowed</t>
+  </si>
+  <si>
+    <t>User Enumeration Not Possible</t>
+  </si>
+  <si>
+    <t>Account Lockout Enabled</t>
+  </si>
+  <si>
+    <t>Multi-Factor Authentication</t>
+  </si>
+  <si>
+    <t>Session Management:</t>
+  </si>
+  <si>
+    <t>Session Fixation</t>
+  </si>
+  <si>
+    <t>Session dies after X minutes</t>
+  </si>
+  <si>
+    <t>Logout Button Works</t>
+  </si>
+  <si>
+    <t>All functions require authentication</t>
   </si>
   <si>
     <t>Miscellaneous</t>
@@ -128,13 +287,19 @@
   </si>
   <si>
     <t>File upload</t>
+  </si>
+  <si>
+    <t>Horizontal Privilege Escalation-IDOR</t>
+  </si>
+  <si>
+    <t>Vertical Privilege Escalation-MFLAC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
+  <fonts count="12">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -148,6 +313,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
@@ -157,6 +323,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="9.0"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <u/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
@@ -165,6 +340,20 @@
       <u/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF1155CC"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF1155CC"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
     </font>
     <font>
       <sz val="10.0"/>
@@ -182,8 +371,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
+        <fgColor theme="0"/>
+        <bgColor theme="0"/>
       </patternFill>
     </fill>
     <fill>
@@ -199,7 +388,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="22">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -218,25 +407,52 @@
     <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" vertical="top"/>
     </xf>
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="top"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -484,13 +700,13 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="s">
-        <v>6</v>
-      </c>
+      <c r="A2" s="5"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="6"/>
+      <c r="E2" s="6" t="s">
+        <v>6</v>
+      </c>
       <c r="F2" s="7" t="s">
         <v>7</v>
       </c>
@@ -502,144 +718,348 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="6"/>
+      <c r="E3" s="8"/>
     </row>
     <row r="4">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="10" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="9" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="11" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="9" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="11" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="9" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="11" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="9" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="11" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="9" t="s">
         <v>24</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="11" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="3" t="s">
         <v>27</v>
       </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
     </row>
     <row r="12">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="13" t="s">
         <v>28</v>
       </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="13">
-      <c r="A13" s="7" t="s">
-        <v>29</v>
+      <c r="A13" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="4" t="s">
-        <v>30</v>
+      <c r="A15" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="7" t="s">
-        <v>31</v>
+      <c r="A16" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="7" t="s">
-        <v>32</v>
-      </c>
+      <c r="A17" s="13"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
     </row>
     <row r="19">
-      <c r="A19" s="4" t="s">
-        <v>33</v>
+      <c r="A19" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="E21" s="18" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="4" t="s">
-        <v>35</v>
+      <c r="A22" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="E22" s="20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E23" s="20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="13" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="4" t="s">
-        <v>36</v>
+      <c r="A28" s="8" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="12" t="s">
-        <v>37</v>
+      <c r="A29" s="13" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="7" t="s">
-        <v>38</v>
+      <c r="A30" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="8"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="8"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="8"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="21" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="7" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -650,7 +1070,17 @@
     <hyperlink r:id="rId4" ref="E7"/>
     <hyperlink r:id="rId5" ref="E8"/>
     <hyperlink r:id="rId6" ref="E9"/>
+    <hyperlink r:id="rId7" ref="E12"/>
+    <hyperlink r:id="rId8" ref="E13"/>
+    <hyperlink r:id="rId9" ref="E14"/>
+    <hyperlink r:id="rId10" ref="E15"/>
+    <hyperlink r:id="rId11" location="heading-exploitable-cors-cases" ref="E16"/>
+    <hyperlink r:id="rId12" ref="E19"/>
+    <hyperlink r:id="rId13" ref="E20"/>
+    <hyperlink r:id="rId14" ref="E21"/>
+    <hyperlink r:id="rId15" ref="E22"/>
+    <hyperlink r:id="rId16" ref="E23"/>
   </hyperlinks>
-  <drawing r:id="rId7"/>
+  <drawing r:id="rId17"/>
 </worksheet>
 </file>
</xml_diff>